<commit_message>
Profitability Over Time Documented
</commit_message>
<xml_diff>
--- a/Project/ProjectWork_BufferDays.xlsx
+++ b/Project/ProjectWork_BufferDays.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudiu\Desktop\Programming\MaxMinSales\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039E0D16-E3A9-4026-A13F-0EEAC9577D25}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA15D5F-658B-4E73-822E-86817FB11D45}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23040" yWindow="540" windowWidth="21600" windowHeight="11388" xr2:uid="{155C7FD5-DD5B-4F41-A8A7-38E748E8A471}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{155C7FD5-DD5B-4F41-A8A7-38E748E8A471}"/>
   </bookViews>
   <sheets>
     <sheet name="Buffer Days Plan" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="139">
   <si>
     <t>Buffer day 01 (session 04)</t>
   </si>
@@ -746,15 +746,48 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -765,39 +798,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1116,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656FA391-C048-4106-9E02-73AAE8E24D0B}">
   <dimension ref="A2:E127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,11 +1131,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
       <c r="E2" s="1" t="s">
         <v>137</v>
       </c>
@@ -1155,10 +1155,10 @@
       <c r="B4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="34">
+      <c r="C4" s="45">
         <v>1</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="47" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1166,8 +1166,8 @@
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="36"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="47"/>
       <c r="E5" s="1" t="s">
         <v>138</v>
       </c>
@@ -1176,8 +1176,8 @@
       <c r="B6" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="36"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="47"/>
       <c r="E6" s="1" t="s">
         <v>138</v>
       </c>
@@ -1186,8 +1186,8 @@
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="36"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="47"/>
       <c r="E7" s="1" t="s">
         <v>138</v>
       </c>
@@ -1196,8 +1196,8 @@
       <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="37"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="48"/>
       <c r="E8" s="1" t="s">
         <v>138</v>
       </c>
@@ -1213,10 +1213,10 @@
       <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="34">
+      <c r="C10" s="45">
         <v>2</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="45">
         <v>6</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -1227,8 +1227,8 @@
       <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
       <c r="E11" s="1" t="s">
         <v>138</v>
       </c>
@@ -1237,8 +1237,8 @@
       <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
       <c r="E12" s="1" t="s">
         <v>138</v>
       </c>
@@ -1247,8 +1247,8 @@
       <c r="B13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
       <c r="E13" s="1" t="s">
         <v>138</v>
       </c>
@@ -1257,8 +1257,8 @@
       <c r="B14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
       <c r="E14" s="1" t="s">
         <v>138</v>
       </c>
@@ -1268,8 +1268,8 @@
       <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
       <c r="E15" s="1" t="s">
         <v>138</v>
       </c>
@@ -1278,8 +1278,8 @@
       <c r="B16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
       <c r="E16" s="1" t="s">
         <v>138</v>
       </c>
@@ -1288,8 +1288,8 @@
       <c r="B17" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
       <c r="E17" s="1" t="s">
         <v>138</v>
       </c>
@@ -1298,10 +1298,10 @@
       <c r="B18" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="31">
+      <c r="C18" s="43">
         <v>3</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="43" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1309,8 +1309,8 @@
       <c r="B19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
       <c r="E19" s="1" t="s">
         <v>138</v>
       </c>
@@ -1319,8 +1319,8 @@
       <c r="B20" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
       <c r="E20" s="1" t="s">
         <v>138</v>
       </c>
@@ -1329,8 +1329,8 @@
       <c r="B21" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
       <c r="E21" s="1" t="s">
         <v>138</v>
       </c>
@@ -1339,8 +1339,8 @@
       <c r="B22" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
       <c r="E22" s="1" t="s">
         <v>138</v>
       </c>
@@ -1349,8 +1349,8 @@
       <c r="B23" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
       <c r="E23" s="1" t="s">
         <v>138</v>
       </c>
@@ -1359,8 +1359,8 @@
       <c r="B24" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
       <c r="E24" s="1" t="s">
         <v>138</v>
       </c>
@@ -1369,8 +1369,8 @@
       <c r="B25" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
       <c r="E25" s="1" t="s">
         <v>138</v>
       </c>
@@ -1379,43 +1379,43 @@
       <c r="B26" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
       <c r="E31" s="1" t="s">
         <v>138</v>
       </c>
@@ -1424,8 +1424,8 @@
       <c r="B32" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
       <c r="E32" s="1" t="s">
         <v>138</v>
       </c>
@@ -1434,8 +1434,8 @@
       <c r="B33" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
       <c r="E33" s="1" t="s">
         <v>138</v>
       </c>
@@ -1444,8 +1444,8 @@
       <c r="B34" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
       <c r="E34" s="1" t="s">
         <v>138</v>
       </c>
@@ -1454,8 +1454,8 @@
       <c r="B35" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="43"/>
       <c r="E35" s="1" t="s">
         <v>138</v>
       </c>
@@ -1464,134 +1464,158 @@
       <c r="B36" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="43"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="43"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="43"/>
+      <c r="E52" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="31"/>
-      <c r="D53" s="31"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="43"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="43"/>
       <c r="E54" s="1" t="s">
         <v>138</v>
       </c>
@@ -1600,8 +1624,8 @@
       <c r="B55" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C55" s="31"/>
-      <c r="D55" s="31"/>
+      <c r="C55" s="43"/>
+      <c r="D55" s="43"/>
       <c r="E55" s="1" t="s">
         <v>138</v>
       </c>
@@ -1610,22 +1634,25 @@
       <c r="B56" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C56" s="31"/>
-      <c r="D56" s="31"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="57" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C57" s="32"/>
-      <c r="D57" s="32"/>
+      <c r="C57" s="44"/>
+      <c r="D57" s="44"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="33" t="s">
+      <c r="B59" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C59" s="33"/>
-      <c r="D59" s="33"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
@@ -1642,10 +1669,10 @@
       <c r="B61" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C61" s="41" t="s">
+      <c r="C61" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="D61" s="43" t="s">
+      <c r="D61" s="37" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1653,250 +1680,286 @@
       <c r="B62" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C62" s="41"/>
-      <c r="D62" s="43"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C63" s="41"/>
-      <c r="D63" s="43"/>
+      <c r="C63" s="35"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C64" s="41"/>
-      <c r="D64" s="43"/>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C64" s="35"/>
+      <c r="D64" s="37"/>
+      <c r="E64" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C65" s="41"/>
-      <c r="D65" s="43"/>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C65" s="35"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C66" s="41"/>
-      <c r="D66" s="43"/>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C66" s="35"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C67" s="41"/>
-      <c r="D67" s="43"/>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C67" s="35"/>
+      <c r="D67" s="37"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C68" s="41"/>
-      <c r="D68" s="43"/>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C68" s="35"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C69" s="41"/>
-      <c r="D69" s="43"/>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C69" s="35"/>
+      <c r="D69" s="37"/>
+      <c r="E69" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C70" s="41"/>
-      <c r="D70" s="43"/>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C70" s="35"/>
+      <c r="D70" s="37"/>
+      <c r="E70" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C71" s="41"/>
-      <c r="D71" s="43"/>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C71" s="35"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C72" s="41"/>
-      <c r="D72" s="43"/>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C72" s="35"/>
+      <c r="D72" s="37"/>
+      <c r="E72" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="41"/>
-      <c r="D73" s="43"/>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C73" s="35"/>
+      <c r="D73" s="37"/>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C74" s="41"/>
-      <c r="D74" s="43"/>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C74" s="35"/>
+      <c r="D74" s="37"/>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="41"/>
-      <c r="D75" s="43"/>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C75" s="35"/>
+      <c r="D75" s="37"/>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C76" s="41"/>
-      <c r="D76" s="43"/>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C76" s="35"/>
+      <c r="D76" s="37"/>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C77" s="41"/>
-      <c r="D77" s="43"/>
-    </row>
-    <row r="78" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="35"/>
+      <c r="D77" s="37"/>
+      <c r="E77" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C78" s="42"/>
-      <c r="D78" s="44"/>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C78" s="36"/>
+      <c r="D78" s="38"/>
+      <c r="E78" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="C79" s="45">
+      <c r="C79" s="39">
         <v>7</v>
       </c>
-      <c r="D79" s="48">
+      <c r="D79" s="42">
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C80" s="46"/>
-      <c r="D80" s="43"/>
+      <c r="C80" s="40"/>
+      <c r="D80" s="37"/>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C81" s="46"/>
-      <c r="D81" s="43"/>
+      <c r="C81" s="40"/>
+      <c r="D81" s="37"/>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C82" s="46"/>
-      <c r="D82" s="43"/>
+      <c r="C82" s="40"/>
+      <c r="D82" s="37"/>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C83" s="46"/>
-      <c r="D83" s="43"/>
+      <c r="C83" s="40"/>
+      <c r="D83" s="37"/>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C84" s="46"/>
-      <c r="D84" s="43"/>
+      <c r="C84" s="40"/>
+      <c r="D84" s="37"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C85" s="46"/>
-      <c r="D85" s="43"/>
+      <c r="C85" s="40"/>
+      <c r="D85" s="37"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C86" s="46"/>
-      <c r="D86" s="43"/>
+      <c r="C86" s="40"/>
+      <c r="D86" s="37"/>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C87" s="46"/>
-      <c r="D87" s="43"/>
+      <c r="C87" s="40"/>
+      <c r="D87" s="37"/>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C88" s="46"/>
-      <c r="D88" s="43"/>
+      <c r="C88" s="40"/>
+      <c r="D88" s="37"/>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C89" s="46"/>
-      <c r="D89" s="43"/>
+      <c r="C89" s="40"/>
+      <c r="D89" s="37"/>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C90" s="46"/>
-      <c r="D90" s="43"/>
+      <c r="C90" s="40"/>
+      <c r="D90" s="37"/>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C91" s="46"/>
-      <c r="D91" s="43"/>
+      <c r="C91" s="40"/>
+      <c r="D91" s="37"/>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C92" s="46"/>
-      <c r="D92" s="43"/>
+      <c r="C92" s="40"/>
+      <c r="D92" s="37"/>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C93" s="46"/>
-      <c r="D93" s="43"/>
+      <c r="C93" s="40"/>
+      <c r="D93" s="37"/>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C94" s="46"/>
-      <c r="D94" s="43"/>
+      <c r="C94" s="40"/>
+      <c r="D94" s="37"/>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C95" s="46"/>
-      <c r="D95" s="43"/>
+      <c r="C95" s="40"/>
+      <c r="D95" s="37"/>
     </row>
     <row r="96" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B96" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C96" s="47"/>
-      <c r="D96" s="44"/>
+      <c r="C96" s="41"/>
+      <c r="D96" s="38"/>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="16"/>
@@ -1904,11 +1967,11 @@
       <c r="D97" s="17"/>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="33" t="s">
+      <c r="B98" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="C98" s="33"/>
-      <c r="D98" s="33"/>
+      <c r="C98" s="34"/>
+      <c r="D98" s="34"/>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
@@ -1925,10 +1988,10 @@
       <c r="B100" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="C100" s="38">
+      <c r="C100" s="31">
         <v>9</v>
       </c>
-      <c r="D100" s="38" t="s">
+      <c r="D100" s="31" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1936,150 +1999,150 @@
       <c r="B101" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C101" s="38"/>
-      <c r="D101" s="38"/>
+      <c r="C101" s="31"/>
+      <c r="D101" s="31"/>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C102" s="38"/>
-      <c r="D102" s="38"/>
+      <c r="C102" s="31"/>
+      <c r="D102" s="31"/>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C103" s="38"/>
-      <c r="D103" s="38"/>
+      <c r="C103" s="31"/>
+      <c r="D103" s="31"/>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C104" s="38"/>
-      <c r="D104" s="38"/>
+      <c r="C104" s="31"/>
+      <c r="D104" s="31"/>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C105" s="38"/>
-      <c r="D105" s="38"/>
+      <c r="C105" s="31"/>
+      <c r="D105" s="31"/>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C106" s="38"/>
-      <c r="D106" s="38"/>
+      <c r="C106" s="31"/>
+      <c r="D106" s="31"/>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C107" s="38"/>
-      <c r="D107" s="38"/>
+      <c r="C107" s="31"/>
+      <c r="D107" s="31"/>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C108" s="38"/>
-      <c r="D108" s="38"/>
+      <c r="C108" s="31"/>
+      <c r="D108" s="31"/>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C109" s="38"/>
-      <c r="D109" s="38"/>
+      <c r="C109" s="31"/>
+      <c r="D109" s="31"/>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C110" s="38"/>
-      <c r="D110" s="38"/>
+      <c r="C110" s="31"/>
+      <c r="D110" s="31"/>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C111" s="38"/>
-      <c r="D111" s="38"/>
+      <c r="C111" s="31"/>
+      <c r="D111" s="31"/>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="C112" s="38"/>
-      <c r="D112" s="38"/>
+      <c r="C112" s="31"/>
+      <c r="D112" s="31"/>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C113" s="38"/>
-      <c r="D113" s="38"/>
+      <c r="C113" s="31"/>
+      <c r="D113" s="31"/>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C114" s="38"/>
-      <c r="D114" s="38"/>
+      <c r="C114" s="31"/>
+      <c r="D114" s="31"/>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C115" s="38"/>
-      <c r="D115" s="38"/>
+      <c r="C115" s="31"/>
+      <c r="D115" s="31"/>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C116" s="38"/>
-      <c r="D116" s="38"/>
+      <c r="C116" s="31"/>
+      <c r="D116" s="31"/>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C117" s="38"/>
-      <c r="D117" s="38"/>
+      <c r="C117" s="31"/>
+      <c r="D117" s="31"/>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C118" s="38"/>
-      <c r="D118" s="38"/>
+      <c r="C118" s="31"/>
+      <c r="D118" s="31"/>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="C119" s="38"/>
-      <c r="D119" s="38"/>
+      <c r="C119" s="31"/>
+      <c r="D119" s="31"/>
     </row>
     <row r="120" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B120" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="C120" s="39"/>
-      <c r="D120" s="39"/>
+      <c r="C120" s="32"/>
+      <c r="D120" s="32"/>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="C121" s="40">
+      <c r="C121" s="33">
         <v>10</v>
       </c>
-      <c r="D121" s="40" t="s">
+      <c r="D121" s="33" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2087,46 +2150,53 @@
       <c r="B122" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C122" s="38"/>
-      <c r="D122" s="38"/>
+      <c r="C122" s="31"/>
+      <c r="D122" s="31"/>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C123" s="38"/>
-      <c r="D123" s="38"/>
+      <c r="C123" s="31"/>
+      <c r="D123" s="31"/>
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C124" s="38"/>
-      <c r="D124" s="38"/>
+      <c r="C124" s="31"/>
+      <c r="D124" s="31"/>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="C125" s="38"/>
-      <c r="D125" s="38"/>
+      <c r="C125" s="31"/>
+      <c r="D125" s="31"/>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="C126" s="38"/>
-      <c r="D126" s="38"/>
+      <c r="C126" s="31"/>
+      <c r="D126" s="31"/>
     </row>
     <row r="127" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B127" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C127" s="39"/>
-      <c r="D127" s="39"/>
+      <c r="C127" s="32"/>
+      <c r="D127" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C18:C57"/>
+    <mergeCell ref="D18:D57"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="C4:C8"/>
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="C10:C17"/>
+    <mergeCell ref="D10:D17"/>
     <mergeCell ref="C100:C120"/>
     <mergeCell ref="D100:D120"/>
     <mergeCell ref="C121:C127"/>
@@ -2137,13 +2207,6 @@
     <mergeCell ref="C79:C96"/>
     <mergeCell ref="D79:D96"/>
     <mergeCell ref="B98:D98"/>
-    <mergeCell ref="C18:C57"/>
-    <mergeCell ref="D18:D57"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="C4:C8"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="C10:C17"/>
-    <mergeCell ref="D10:D17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B6" location="'Analytics_ Facts_Dimensions'!A1" display="Choose Analytics /Facts/Dimensions (find the table in the next sheet)" xr:uid="{B27A2A48-0C3F-4EB9-B72F-64F645DD2FD9}"/>
@@ -2233,6 +2296,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100321BE94CFD421B478088255E2A1AF3E3" ma:contentTypeVersion="13" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="23e035453a8c666fd46abd439f0a5200">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0511ba9c-287a-4da1-9b3d-dae995630eb0" xmlns:ns4="e96f1435-982b-4d55-a247-affd85372afe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24a4ced9b2a06340f3c1ca5f9e85d693" ns3:_="" ns4:_="">
     <xsd:import namespace="0511ba9c-287a-4da1-9b3d-dae995630eb0"/>
@@ -2455,15 +2527,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A010B317-73FD-4C50-AA10-14E9D0D8789B}">
   <ds:schemaRefs>
@@ -2482,6 +2545,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{102B36DA-40DA-497A-AAA8-AA20404F5F17}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{959ACB82-3975-434E-9A46-FAC8D497B785}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2498,12 +2569,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{102B36DA-40DA-497A-AAA8-AA20404F5F17}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
SSRS part for payment method done
</commit_message>
<xml_diff>
--- a/Project/ProjectWork_BufferDays.xlsx
+++ b/Project/ProjectWork_BufferDays.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudiu\Desktop\Programming\MaxMinSales\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA15D5F-658B-4E73-822E-86817FB11D45}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D561DD-17C4-4F81-9BE2-388E82BD88B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{155C7FD5-DD5B-4F41-A8A7-38E748E8A471}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{155C7FD5-DD5B-4F41-A8A7-38E748E8A471}"/>
   </bookViews>
   <sheets>
     <sheet name="Buffer Days Plan" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="139">
   <si>
     <t>Buffer day 01 (session 04)</t>
   </si>
@@ -746,6 +746,27 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -755,9 +776,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -780,24 +798,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1116,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656FA391-C048-4106-9E02-73AAE8E24D0B}">
   <dimension ref="A2:E127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E111" sqref="E111"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,11 +1131,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="1" t="s">
         <v>137</v>
       </c>
@@ -1155,10 +1155,10 @@
       <c r="B4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="34">
         <v>1</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="36" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1166,8 +1166,8 @@
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="47"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="36"/>
       <c r="E5" s="1" t="s">
         <v>138</v>
       </c>
@@ -1176,8 +1176,8 @@
       <c r="B6" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="47"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="36"/>
       <c r="E6" s="1" t="s">
         <v>138</v>
       </c>
@@ -1186,8 +1186,8 @@
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="47"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="36"/>
       <c r="E7" s="1" t="s">
         <v>138</v>
       </c>
@@ -1196,8 +1196,8 @@
       <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="48"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="37"/>
       <c r="E8" s="1" t="s">
         <v>138</v>
       </c>
@@ -1213,10 +1213,10 @@
       <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="45">
+      <c r="C10" s="34">
         <v>2</v>
       </c>
-      <c r="D10" s="45">
+      <c r="D10" s="34">
         <v>6</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -1227,8 +1227,8 @@
       <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="1" t="s">
         <v>138</v>
       </c>
@@ -1237,8 +1237,8 @@
       <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="1" t="s">
         <v>138</v>
       </c>
@@ -1247,8 +1247,8 @@
       <c r="B13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="1" t="s">
         <v>138</v>
       </c>
@@ -1257,8 +1257,8 @@
       <c r="B14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="1" t="s">
         <v>138</v>
       </c>
@@ -1268,8 +1268,8 @@
       <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
       <c r="E15" s="1" t="s">
         <v>138</v>
       </c>
@@ -1278,8 +1278,8 @@
       <c r="B16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="1" t="s">
         <v>138</v>
       </c>
@@ -1288,8 +1288,8 @@
       <c r="B17" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
       <c r="E17" s="1" t="s">
         <v>138</v>
       </c>
@@ -1298,10 +1298,10 @@
       <c r="B18" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="43">
+      <c r="C18" s="31">
         <v>3</v>
       </c>
-      <c r="D18" s="43" t="s">
+      <c r="D18" s="31" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1309,8 +1309,8 @@
       <c r="B19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="1" t="s">
         <v>138</v>
       </c>
@@ -1319,8 +1319,8 @@
       <c r="B20" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
       <c r="E20" s="1" t="s">
         <v>138</v>
       </c>
@@ -1329,8 +1329,8 @@
       <c r="B21" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
       <c r="E21" s="1" t="s">
         <v>138</v>
       </c>
@@ -1339,8 +1339,8 @@
       <c r="B22" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
       <c r="E22" s="1" t="s">
         <v>138</v>
       </c>
@@ -1349,8 +1349,8 @@
       <c r="B23" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="1" t="s">
         <v>138</v>
       </c>
@@ -1359,8 +1359,8 @@
       <c r="B24" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
       <c r="E24" s="1" t="s">
         <v>138</v>
       </c>
@@ -1369,8 +1369,8 @@
       <c r="B25" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
       <c r="E25" s="1" t="s">
         <v>138</v>
       </c>
@@ -1379,43 +1379,43 @@
       <c r="B26" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
       <c r="E31" s="1" t="s">
         <v>138</v>
       </c>
@@ -1424,8 +1424,8 @@
       <c r="B32" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
       <c r="E32" s="1" t="s">
         <v>138</v>
       </c>
@@ -1434,8 +1434,8 @@
       <c r="B33" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
       <c r="E33" s="1" t="s">
         <v>138</v>
       </c>
@@ -1444,8 +1444,8 @@
       <c r="B34" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
       <c r="E34" s="1" t="s">
         <v>138</v>
       </c>
@@ -1454,8 +1454,8 @@
       <c r="B35" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
       <c r="E35" s="1" t="s">
         <v>138</v>
       </c>
@@ -1464,8 +1464,8 @@
       <c r="B36" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
       <c r="E36" s="1" t="s">
         <v>138</v>
       </c>
@@ -1474,8 +1474,8 @@
       <c r="B37" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
       <c r="E37" s="1" t="s">
         <v>138</v>
       </c>
@@ -1484,29 +1484,29 @@
       <c r="B38" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="43"/>
-      <c r="D40" s="43"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
       <c r="E41" s="1" t="s">
         <v>138</v>
       </c>
@@ -1515,8 +1515,8 @@
       <c r="B42" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="43"/>
-      <c r="D42" s="43"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
       <c r="E42" s="1" t="s">
         <v>138</v>
       </c>
@@ -1525,8 +1525,8 @@
       <c r="B43" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
       <c r="E43" s="1" t="s">
         <v>138</v>
       </c>
@@ -1535,29 +1535,29 @@
       <c r="B44" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
       <c r="E47" s="1" t="s">
         <v>138</v>
       </c>
@@ -1566,15 +1566,15 @@
       <c r="B48" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="43"/>
-      <c r="D49" s="43"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
       <c r="E49" s="1" t="s">
         <v>138</v>
       </c>
@@ -1583,22 +1583,22 @@
       <c r="B50" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="43"/>
-      <c r="D50" s="43"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C51" s="43"/>
-      <c r="D51" s="43"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="31"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C52" s="43"/>
-      <c r="D52" s="43"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="31"/>
       <c r="E52" s="1" t="s">
         <v>138</v>
       </c>
@@ -1607,15 +1607,15 @@
       <c r="B53" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="43"/>
-      <c r="D53" s="43"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C54" s="43"/>
-      <c r="D54" s="43"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
       <c r="E54" s="1" t="s">
         <v>138</v>
       </c>
@@ -1624,8 +1624,8 @@
       <c r="B55" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C55" s="43"/>
-      <c r="D55" s="43"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
       <c r="E55" s="1" t="s">
         <v>138</v>
       </c>
@@ -1634,8 +1634,8 @@
       <c r="B56" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C56" s="43"/>
-      <c r="D56" s="43"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
       <c r="E56" s="1" t="s">
         <v>138</v>
       </c>
@@ -1644,15 +1644,15 @@
       <c r="B57" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C57" s="44"/>
-      <c r="D57" s="44"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="34" t="s">
+      <c r="B59" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="33"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
@@ -1669,10 +1669,10 @@
       <c r="B61" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C61" s="35" t="s">
+      <c r="C61" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="D61" s="37" t="s">
+      <c r="D61" s="43" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1680,8 +1680,8 @@
       <c r="B62" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C62" s="35"/>
-      <c r="D62" s="37"/>
+      <c r="C62" s="41"/>
+      <c r="D62" s="43"/>
       <c r="E62" s="1" t="s">
         <v>138</v>
       </c>
@@ -1690,8 +1690,8 @@
       <c r="B63" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C63" s="35"/>
-      <c r="D63" s="37"/>
+      <c r="C63" s="41"/>
+      <c r="D63" s="43"/>
       <c r="E63" s="1" t="s">
         <v>138</v>
       </c>
@@ -1700,8 +1700,8 @@
       <c r="B64" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C64" s="35"/>
-      <c r="D64" s="37"/>
+      <c r="C64" s="41"/>
+      <c r="D64" s="43"/>
       <c r="E64" s="1" t="s">
         <v>138</v>
       </c>
@@ -1710,8 +1710,8 @@
       <c r="B65" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C65" s="35"/>
-      <c r="D65" s="37"/>
+      <c r="C65" s="41"/>
+      <c r="D65" s="43"/>
       <c r="E65" s="1" t="s">
         <v>138</v>
       </c>
@@ -1720,8 +1720,8 @@
       <c r="B66" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C66" s="35"/>
-      <c r="D66" s="37"/>
+      <c r="C66" s="41"/>
+      <c r="D66" s="43"/>
       <c r="E66" s="1" t="s">
         <v>138</v>
       </c>
@@ -1730,15 +1730,15 @@
       <c r="B67" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C67" s="35"/>
-      <c r="D67" s="37"/>
+      <c r="C67" s="41"/>
+      <c r="D67" s="43"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C68" s="35"/>
-      <c r="D68" s="37"/>
+      <c r="C68" s="41"/>
+      <c r="D68" s="43"/>
       <c r="E68" s="1" t="s">
         <v>138</v>
       </c>
@@ -1747,8 +1747,8 @@
       <c r="B69" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C69" s="35"/>
-      <c r="D69" s="37"/>
+      <c r="C69" s="41"/>
+      <c r="D69" s="43"/>
       <c r="E69" s="1" t="s">
         <v>138</v>
       </c>
@@ -1757,8 +1757,8 @@
       <c r="B70" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C70" s="35"/>
-      <c r="D70" s="37"/>
+      <c r="C70" s="41"/>
+      <c r="D70" s="43"/>
       <c r="E70" s="1" t="s">
         <v>138</v>
       </c>
@@ -1767,8 +1767,8 @@
       <c r="B71" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C71" s="35"/>
-      <c r="D71" s="37"/>
+      <c r="C71" s="41"/>
+      <c r="D71" s="43"/>
       <c r="E71" s="1" t="s">
         <v>138</v>
       </c>
@@ -1777,8 +1777,8 @@
       <c r="B72" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C72" s="35"/>
-      <c r="D72" s="37"/>
+      <c r="C72" s="41"/>
+      <c r="D72" s="43"/>
       <c r="E72" s="1" t="s">
         <v>138</v>
       </c>
@@ -1787,36 +1787,36 @@
       <c r="B73" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="35"/>
-      <c r="D73" s="37"/>
+      <c r="C73" s="41"/>
+      <c r="D73" s="43"/>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C74" s="35"/>
-      <c r="D74" s="37"/>
+      <c r="C74" s="41"/>
+      <c r="D74" s="43"/>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="35"/>
-      <c r="D75" s="37"/>
+      <c r="C75" s="41"/>
+      <c r="D75" s="43"/>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C76" s="35"/>
-      <c r="D76" s="37"/>
+      <c r="C76" s="41"/>
+      <c r="D76" s="43"/>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C77" s="35"/>
-      <c r="D77" s="37"/>
+      <c r="C77" s="41"/>
+      <c r="D77" s="43"/>
       <c r="E77" s="1" t="s">
         <v>138</v>
       </c>
@@ -1825,8 +1825,8 @@
       <c r="B78" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C78" s="36"/>
-      <c r="D78" s="38"/>
+      <c r="C78" s="42"/>
+      <c r="D78" s="44"/>
       <c r="E78" s="1" t="s">
         <v>138</v>
       </c>
@@ -1835,10 +1835,10 @@
       <c r="B79" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="C79" s="39">
+      <c r="C79" s="45">
         <v>7</v>
       </c>
-      <c r="D79" s="42">
+      <c r="D79" s="48">
         <v>17</v>
       </c>
     </row>
@@ -1846,120 +1846,144 @@
       <c r="B80" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C80" s="40"/>
-      <c r="D80" s="37"/>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C80" s="46"/>
+      <c r="D80" s="43"/>
+      <c r="E80" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C81" s="40"/>
-      <c r="D81" s="37"/>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C81" s="46"/>
+      <c r="D81" s="43"/>
+      <c r="E81" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C82" s="40"/>
-      <c r="D82" s="37"/>
-    </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C82" s="46"/>
+      <c r="D82" s="43"/>
+      <c r="E82" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C83" s="40"/>
-      <c r="D83" s="37"/>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C83" s="46"/>
+      <c r="D83" s="43"/>
+      <c r="E83" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C84" s="40"/>
-      <c r="D84" s="37"/>
-    </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C84" s="46"/>
+      <c r="D84" s="43"/>
+      <c r="E84" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C85" s="40"/>
-      <c r="D85" s="37"/>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C85" s="46"/>
+      <c r="D85" s="43"/>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C86" s="40"/>
-      <c r="D86" s="37"/>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C86" s="46"/>
+      <c r="D86" s="43"/>
+      <c r="E86" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C87" s="40"/>
-      <c r="D87" s="37"/>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C87" s="46"/>
+      <c r="D87" s="43"/>
+      <c r="E87" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C88" s="40"/>
-      <c r="D88" s="37"/>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C88" s="46"/>
+      <c r="D88" s="43"/>
+      <c r="E88" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C89" s="40"/>
-      <c r="D89" s="37"/>
-    </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C89" s="46"/>
+      <c r="D89" s="43"/>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C90" s="40"/>
-      <c r="D90" s="37"/>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C90" s="46"/>
+      <c r="D90" s="43"/>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C91" s="40"/>
-      <c r="D91" s="37"/>
-    </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C91" s="46"/>
+      <c r="D91" s="43"/>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C92" s="40"/>
-      <c r="D92" s="37"/>
-    </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C92" s="46"/>
+      <c r="D92" s="43"/>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C93" s="40"/>
-      <c r="D93" s="37"/>
-    </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C93" s="46"/>
+      <c r="D93" s="43"/>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C94" s="40"/>
-      <c r="D94" s="37"/>
-    </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C94" s="46"/>
+      <c r="D94" s="43"/>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C95" s="40"/>
-      <c r="D95" s="37"/>
-    </row>
-    <row r="96" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C95" s="46"/>
+      <c r="D95" s="43"/>
+    </row>
+    <row r="96" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B96" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C96" s="41"/>
-      <c r="D96" s="38"/>
+      <c r="C96" s="47"/>
+      <c r="D96" s="44"/>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="16"/>
@@ -1967,11 +1991,11 @@
       <c r="D97" s="17"/>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="34" t="s">
+      <c r="B98" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="C98" s="34"/>
-      <c r="D98" s="34"/>
+      <c r="C98" s="33"/>
+      <c r="D98" s="33"/>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
@@ -1988,10 +2012,10 @@
       <c r="B100" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="C100" s="31">
+      <c r="C100" s="38">
         <v>9</v>
       </c>
-      <c r="D100" s="31" t="s">
+      <c r="D100" s="38" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1999,150 +2023,150 @@
       <c r="B101" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C101" s="31"/>
-      <c r="D101" s="31"/>
+      <c r="C101" s="38"/>
+      <c r="D101" s="38"/>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C102" s="31"/>
-      <c r="D102" s="31"/>
+      <c r="C102" s="38"/>
+      <c r="D102" s="38"/>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C103" s="31"/>
-      <c r="D103" s="31"/>
+      <c r="C103" s="38"/>
+      <c r="D103" s="38"/>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C104" s="31"/>
-      <c r="D104" s="31"/>
+      <c r="C104" s="38"/>
+      <c r="D104" s="38"/>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C105" s="31"/>
-      <c r="D105" s="31"/>
+      <c r="C105" s="38"/>
+      <c r="D105" s="38"/>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C106" s="31"/>
-      <c r="D106" s="31"/>
+      <c r="C106" s="38"/>
+      <c r="D106" s="38"/>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C107" s="31"/>
-      <c r="D107" s="31"/>
+      <c r="C107" s="38"/>
+      <c r="D107" s="38"/>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C108" s="31"/>
-      <c r="D108" s="31"/>
+      <c r="C108" s="38"/>
+      <c r="D108" s="38"/>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C109" s="31"/>
-      <c r="D109" s="31"/>
+      <c r="C109" s="38"/>
+      <c r="D109" s="38"/>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C110" s="31"/>
-      <c r="D110" s="31"/>
+      <c r="C110" s="38"/>
+      <c r="D110" s="38"/>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C111" s="31"/>
-      <c r="D111" s="31"/>
+      <c r="C111" s="38"/>
+      <c r="D111" s="38"/>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="C112" s="31"/>
-      <c r="D112" s="31"/>
+      <c r="C112" s="38"/>
+      <c r="D112" s="38"/>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C113" s="31"/>
-      <c r="D113" s="31"/>
+      <c r="C113" s="38"/>
+      <c r="D113" s="38"/>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C114" s="31"/>
-      <c r="D114" s="31"/>
+      <c r="C114" s="38"/>
+      <c r="D114" s="38"/>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C115" s="31"/>
-      <c r="D115" s="31"/>
+      <c r="C115" s="38"/>
+      <c r="D115" s="38"/>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C116" s="31"/>
-      <c r="D116" s="31"/>
+      <c r="C116" s="38"/>
+      <c r="D116" s="38"/>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C117" s="31"/>
-      <c r="D117" s="31"/>
+      <c r="C117" s="38"/>
+      <c r="D117" s="38"/>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C118" s="31"/>
-      <c r="D118" s="31"/>
+      <c r="C118" s="38"/>
+      <c r="D118" s="38"/>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="C119" s="31"/>
-      <c r="D119" s="31"/>
+      <c r="C119" s="38"/>
+      <c r="D119" s="38"/>
     </row>
     <row r="120" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B120" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="C120" s="32"/>
-      <c r="D120" s="32"/>
+      <c r="C120" s="39"/>
+      <c r="D120" s="39"/>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="C121" s="33">
+      <c r="C121" s="40">
         <v>10</v>
       </c>
-      <c r="D121" s="33" t="s">
+      <c r="D121" s="40" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2150,53 +2174,46 @@
       <c r="B122" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C122" s="31"/>
-      <c r="D122" s="31"/>
+      <c r="C122" s="38"/>
+      <c r="D122" s="38"/>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C123" s="31"/>
-      <c r="D123" s="31"/>
+      <c r="C123" s="38"/>
+      <c r="D123" s="38"/>
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C124" s="31"/>
-      <c r="D124" s="31"/>
+      <c r="C124" s="38"/>
+      <c r="D124" s="38"/>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="C125" s="31"/>
-      <c r="D125" s="31"/>
+      <c r="C125" s="38"/>
+      <c r="D125" s="38"/>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="C126" s="31"/>
-      <c r="D126" s="31"/>
+      <c r="C126" s="38"/>
+      <c r="D126" s="38"/>
     </row>
     <row r="127" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B127" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C127" s="32"/>
-      <c r="D127" s="32"/>
+      <c r="C127" s="39"/>
+      <c r="D127" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C18:C57"/>
-    <mergeCell ref="D18:D57"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="C4:C8"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="C10:C17"/>
-    <mergeCell ref="D10:D17"/>
     <mergeCell ref="C100:C120"/>
     <mergeCell ref="D100:D120"/>
     <mergeCell ref="C121:C127"/>
@@ -2207,6 +2224,13 @@
     <mergeCell ref="C79:C96"/>
     <mergeCell ref="D79:D96"/>
     <mergeCell ref="B98:D98"/>
+    <mergeCell ref="C18:C57"/>
+    <mergeCell ref="D18:D57"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="C4:C8"/>
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="C10:C17"/>
+    <mergeCell ref="D10:D17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B6" location="'Analytics_ Facts_Dimensions'!A1" display="Choose Analytics /Facts/Dimensions (find the table in the next sheet)" xr:uid="{B27A2A48-0C3F-4EB9-B72F-64F645DD2FD9}"/>
@@ -2296,15 +2320,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100321BE94CFD421B478088255E2A1AF3E3" ma:contentTypeVersion="13" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="23e035453a8c666fd46abd439f0a5200">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0511ba9c-287a-4da1-9b3d-dae995630eb0" xmlns:ns4="e96f1435-982b-4d55-a247-affd85372afe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24a4ced9b2a06340f3c1ca5f9e85d693" ns3:_="" ns4:_="">
     <xsd:import namespace="0511ba9c-287a-4da1-9b3d-dae995630eb0"/>
@@ -2527,6 +2542,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A010B317-73FD-4C50-AA10-14E9D0D8789B}">
   <ds:schemaRefs>
@@ -2545,14 +2569,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{102B36DA-40DA-497A-AAA8-AA20404F5F17}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{959ACB82-3975-434E-9A46-FAC8D497B785}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2569,4 +2585,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{102B36DA-40DA-497A-AAA8-AA20404F5F17}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>